<commit_message>
15 Oct 2024 - LV Contacts - Final
</commit_message>
<xml_diff>
--- a/TestData/T1103_CreateNewRelationshipInHoulihanEmployeeDetailPage.xlsx
+++ b/TestData/T1103_CreateNewRelationshipInHoulihanEmployeeDetailPage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16735D8-1DBA-411A-9C50-D2644B9029E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A27BB6-FAB7-4E04-9343-CED71162E8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>CompanyName</t>
   </si>
@@ -41,12 +41,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>Houlihan</t>
-  </si>
-  <si>
-    <t>StdUser</t>
-  </si>
-  <si>
     <t>Houlihan Contact</t>
   </si>
   <si>
@@ -59,29 +53,53 @@
     <t>External Contact</t>
   </si>
   <si>
-    <t>Test Houlihan</t>
-  </si>
-  <si>
     <t>Business</t>
   </si>
   <si>
     <t>High</t>
   </si>
   <si>
-    <t>Test External</t>
+    <t>Amanda Donovan</t>
+  </si>
+  <si>
+    <t>CF Financial</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>(541) 754-3010</t>
+  </si>
+  <si>
+    <t>ExtContact</t>
+  </si>
+  <si>
+    <t>Test ExtContact</t>
+  </si>
+  <si>
+    <t>TestExtContact@email.com</t>
+  </si>
+  <si>
+    <t>ContactType</t>
   </si>
   <si>
     <t>StandardTestCompany</t>
   </si>
   <si>
-    <t>Ayati Arvind</t>
+    <t>Houlihan Employee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +111,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,14 +141,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -401,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -412,9 +442,13 @@
     <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,19 +458,46 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{D750CDB3-057E-44C6-BFF5-8EF47FB9C0B1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -445,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,13 +518,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -475,13 +536,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
@@ -489,30 +550,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>